<commit_message>
[week6 day4][work] Start the QOS code migration with learning. [study] complete the space vector [physical status] 4 the spirit is slowly healing
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>xy</t>
   </si>
@@ -28,59 +28,107 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>超级精神</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很精神</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有一点萎靡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>萎靡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>疲惫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一点点疲惫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非常疲惫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很疲惫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身心俱疲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旨在找到自己身体什么时候更疲劳，怀疑自己的身体像月经一样有规律</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>睡觉时间，以10点半为起点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>心情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">疲劳状态 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>完全学不进去</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超级精神</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很精神</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>精神</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有一点萎靡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>萎靡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>疲惫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>一点点疲惫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>非常疲惫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>很疲惫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>身心俱疲</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>旨在找到自己身体什么时候更疲劳，怀疑自己的身体像月经一样有规律</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>睡觉时间，以10点半为起点</t>
+    <t>非常好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好得不能再好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神得不能再精神</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有点差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不太好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>很差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非常差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>崩溃</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -158,12 +206,19 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -238,17 +293,17 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>身体状态!$B$1</c:f>
+              <c:f>身体状态!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>xy</c:v>
+                  <c:v>睡觉时间，以10点半为起点</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -283,23 +338,29 @@
                 <c:pt idx="2">
                   <c:v>43166</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43167</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>身体状态!$B$2:$B$4</c:f>
+              <c:f>身体状态!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,11 +376,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>身体状态!$C$1</c:f>
+              <c:f>身体状态!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>睡觉时间，以10点半为起点</c:v>
+                  <c:v>心情</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -339,23 +400,86 @@
                 <c:pt idx="2">
                   <c:v>43166</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43167</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>身体状态!$C$2:$C$4</c:f>
+              <c:f>身体状态!$D$2:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>身体状态!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>xy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>身体状态!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy/m/d</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>43164</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43165</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43166</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>身体状态!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,11 +489,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="62464000"/>
-        <c:axId val="62465920"/>
+        <c:axId val="84882560"/>
+        <c:axId val="84884480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62464000"/>
+        <c:axId val="84882560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,14 +569,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62465920"/>
+        <c:crossAx val="84884480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62465920"/>
+        <c:axId val="84884480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +666,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62464000"/>
+        <c:crossAx val="84882560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -619,7 +743,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -645,7 +769,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -667,11 +791,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:C23" totalsRowCount="1" headerRowDxfId="6" dataDxfId="5" totalsRowDxfId="4">
-  <autoFilter ref="B1:C22"/>
-  <tableColumns count="2">
-    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1"/>
-    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="2" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:D23" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6">
+  <autoFilter ref="B1:D22">
+    <filterColumn colId="2"/>
+  </autoFilter>
+  <tableColumns count="3">
+    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="心情" dataDxfId="3" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -932,7 +1059,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -949,14 +1076,14 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.875" style="3" customWidth="1"/>
     <col min="3" max="3" width="25.625" customWidth="1"/>
     <col min="5" max="6" width="6.125" customWidth="1"/>
     <col min="7" max="7" width="18.75" customWidth="1"/>
     <col min="8" max="8" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -964,10 +1091,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>43164</v>
       </c>
@@ -977,8 +1107,11 @@
       <c r="C2" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>43165</v>
       </c>
@@ -988,8 +1121,11 @@
       <c r="C3" s="4">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>43166</v>
       </c>
@@ -999,107 +1135,140 @@
       <c r="C4" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>43167</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
+        <v>19</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="3" t="s">
-        <v>2</v>
+      <c r="C28" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1107,7 +1276,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1115,7 +1287,10 @@
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1123,10 +1298,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1140,63 +1318,87 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>4</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>5</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>7</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>8</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>9</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>10</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[week6 day5] Complete the code error correction of cap resource management and complete the adaptation of the action code interface in QOS. [physical status] 3 today is nice day
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -341,6 +341,9 @@
                 <c:pt idx="3">
                   <c:v>43167</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>43168</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -361,6 +364,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -403,6 +409,9 @@
                 <c:pt idx="3">
                   <c:v>43167</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>43168</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -422,6 +431,9 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -460,6 +472,9 @@
                 <c:pt idx="3">
                   <c:v>43167</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>43168</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -481,6 +496,9 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -489,11 +507,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="84882560"/>
-        <c:axId val="84884480"/>
+        <c:axId val="58961920"/>
+        <c:axId val="58963840"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="84882560"/>
+        <c:axId val="58961920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,14 +587,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84884480"/>
+        <c:crossAx val="58963840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="84884480"/>
+        <c:axId val="58963840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,7 +684,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84882560"/>
+        <c:crossAx val="58961920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -743,7 +761,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -769,7 +787,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1059,7 +1077,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1070,7 +1088,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1154,10 +1172,18 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="2">
+        <v>43168</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
@@ -1258,7 +1284,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week6 day6] I'm in a not bad mood today. I hope I can clam down and complete the adaptation of QOS code
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -344,6 +344,9 @@
                 <c:pt idx="4">
                   <c:v>43168</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>43169</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -367,6 +370,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,6 +418,9 @@
                 <c:pt idx="4">
                   <c:v>43168</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>43169</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -434,6 +443,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -475,6 +487,9 @@
                 <c:pt idx="4">
                   <c:v>43168</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>43169</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -499,6 +514,9 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -507,11 +525,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="58961920"/>
-        <c:axId val="58963840"/>
+        <c:axId val="83668992"/>
+        <c:axId val="83670912"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="58961920"/>
+        <c:axId val="83668992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -587,14 +605,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58963840"/>
+        <c:crossAx val="83670912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="58963840"/>
+        <c:axId val="83670912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -684,7 +702,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58961920"/>
+        <c:crossAx val="83668992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -761,7 +779,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -787,7 +805,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1077,7 +1095,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1088,7 +1106,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1186,10 +1204,18 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="2">
+        <v>43169</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2"/>
@@ -1284,7 +1310,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[physical status] In general, the current state of mind is stable and mood is stable too.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>xy</t>
   </si>
@@ -130,6 +130,13 @@
   <si>
     <t>崩溃</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 这天晚上跟她生闷气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>列1</t>
   </si>
 </sst>
 </file>
@@ -187,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -202,16 +209,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -221,8 +232,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -292,8 +309,8 @@
     </c:title>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
@@ -347,6 +364,12 @@
                 <c:pt idx="5">
                   <c:v>43169</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>43170</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43171</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -372,6 +395,12 @@
                   <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -397,6 +426,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>身体状态!$A$2:$A$22</c:f>
@@ -420,6 +452,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43170</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -447,6 +485,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,6 +510,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>身体状态!$A$2:$A$22</c:f>
@@ -489,6 +536,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43170</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,23 +570,26 @@
                 <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls>
-          <c:showVal val="1"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:axId val="83668992"/>
-        <c:axId val="83670912"/>
-      </c:lineChart>
-      <c:dateAx>
-        <c:axId val="83668992"/>
+        <c:axId val="44135168"/>
+        <c:axId val="73971584"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="44135168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -605,14 +661,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83670912"/>
+        <c:crossAx val="73971584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="83670912"/>
+        <c:axId val="73971584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +758,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83668992"/>
+        <c:crossAx val="44135168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -728,7 +784,7 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr rtl="0">
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -779,7 +835,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -789,16 +845,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>276227</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>352427</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -827,14 +883,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:D23" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6">
-  <autoFilter ref="B1:D22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:E23" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+  <autoFilter ref="B1:E22">
     <filterColumn colId="2"/>
+    <filterColumn colId="3"/>
   </autoFilter>
-  <tableColumns count="3">
-    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="2"/>
-    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="2" name="心情" dataDxfId="3" totalsRowDxfId="0"/>
+  <tableColumns count="4">
+    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="心情" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="列1" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1103,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1114,12 +1172,13 @@
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.875" style="3" customWidth="1"/>
     <col min="3" max="3" width="25.625" customWidth="1"/>
-    <col min="5" max="6" width="6.125" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="6.125" customWidth="1"/>
     <col min="7" max="7" width="18.75" customWidth="1"/>
     <col min="8" max="8" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1132,8 +1191,11 @@
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>43164</v>
       </c>
@@ -1146,8 +1208,9 @@
       <c r="D2" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>43165</v>
       </c>
@@ -1160,8 +1223,9 @@
       <c r="D3" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>43166</v>
       </c>
@@ -1174,8 +1238,9 @@
       <c r="D4" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>43167</v>
       </c>
@@ -1188,8 +1253,9 @@
       <c r="D5" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>43168</v>
       </c>
@@ -1202,8 +1268,9 @@
       <c r="D6" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>43169</v>
       </c>
@@ -1216,104 +1283,139 @@
       <c r="D7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>43170</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>43171</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="28" spans="1:11">
       <c r="B28" s="3" t="s">
@@ -1354,9 +1456,6 @@
       </c>
       <c r="C31" t="s">
         <v>18</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1451,6 +1550,11 @@
       </c>
       <c r="C39" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="85.5">
+      <c r="A41" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[week7 day2][plan] the main plan today is to complete the compilation of all the code, and another chapter of mathematics learning. In the mood, continuous stable status
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -218,11 +218,13 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -232,14 +234,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -370,6 +370,9 @@
                 <c:pt idx="7">
                   <c:v>43171</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>43172</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -402,6 +405,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -459,6 +465,9 @@
                 <c:pt idx="7">
                   <c:v>43171</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>43172</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -490,6 +499,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -543,6 +555,9 @@
                 <c:pt idx="7">
                   <c:v>43171</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>43172</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -576,15 +591,18 @@
                 <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="44135168"/>
-        <c:axId val="73971584"/>
+        <c:axId val="60014592"/>
+        <c:axId val="60016512"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="44135168"/>
+        <c:axId val="60014592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,14 +679,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73971584"/>
+        <c:crossAx val="60016512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73971584"/>
+        <c:axId val="60016512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +776,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44135168"/>
+        <c:crossAx val="60014592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -835,7 +853,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -861,7 +879,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -889,10 +907,10 @@
     <filterColumn colId="3"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="心情" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="3" name="列1" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="心情" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="3" name="列1" dataDxfId="4" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1153,7 +1171,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1164,7 +1182,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1318,10 +1336,18 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="2">
+        <v>43172</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5">
@@ -1411,7 +1437,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week7 day2-3] yesterday's completion rate was 100%, so hit the card once. [plan] today's main task is to complete the coding and debugging of mac acl in PRS, and to complete daily English and mathematics learning
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -409,6 +409,9 @@
                 <c:pt idx="8">
                   <c:v>2.5</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -504,6 +507,9 @@
                 <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -594,15 +600,18 @@
                 <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="60014592"/>
-        <c:axId val="60016512"/>
+        <c:axId val="73711616"/>
+        <c:axId val="73713536"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="60014592"/>
+        <c:axId val="73711616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -679,14 +688,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60016512"/>
+        <c:crossAx val="73713536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60016512"/>
+        <c:axId val="73713536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,17 +785,10 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60014592"/>
+        <c:crossAx val="73711616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -853,7 +855,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -879,7 +881,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1171,7 +1173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1182,7 +1184,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1352,9 +1354,15 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="4">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5">
@@ -1437,7 +1445,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week7 day5] Today I must study a section of mathematics.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -379,6 +379,9 @@
                 <c:pt idx="10">
                   <c:v>43174</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>43175</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -420,6 +423,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -486,6 +492,9 @@
                 <c:pt idx="10">
                   <c:v>43174</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>43175</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -526,6 +535,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -588,6 +600,9 @@
                 <c:pt idx="10">
                   <c:v>43174</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>43175</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -630,15 +645,18 @@
                 <c:pt idx="10">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="63291392"/>
-        <c:axId val="63293312"/>
+        <c:axId val="62562304"/>
+        <c:axId val="62564224"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="63291392"/>
+        <c:axId val="62562304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -715,14 +733,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63293312"/>
+        <c:crossAx val="62564224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63293312"/>
+        <c:axId val="62564224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +830,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63291392"/>
+        <c:crossAx val="62562304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -882,7 +900,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -908,7 +926,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1200,7 +1218,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1211,7 +1229,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1410,10 +1428,18 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="2">
+        <v>43175</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
@@ -1482,7 +1508,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week7 day6] First of all, ensure that the first chapter os mathematics learning, remaining time to read the QOS code.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>xy</t>
   </si>
@@ -137,6 +137,10 @@
   </si>
   <si>
     <t>列1</t>
+  </si>
+  <si>
+    <t>睡得晚，眼睛有点痛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -382,6 +386,9 @@
                 <c:pt idx="11">
                   <c:v>43175</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>43176</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -426,6 +433,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,6 +505,9 @@
                 <c:pt idx="11">
                   <c:v>43175</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>43176</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -538,6 +551,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -603,6 +619,9 @@
                 <c:pt idx="11">
                   <c:v>43175</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>43176</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -648,15 +667,18 @@
                 <c:pt idx="11">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="62562304"/>
-        <c:axId val="62564224"/>
+        <c:axId val="79867904"/>
+        <c:axId val="79869824"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="62562304"/>
+        <c:axId val="79867904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,14 +755,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62564224"/>
+        <c:crossAx val="79869824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62564224"/>
+        <c:axId val="79869824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +852,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62562304"/>
+        <c:crossAx val="79867904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -900,7 +922,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -926,7 +948,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1218,7 +1240,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1229,7 +1251,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1443,11 +1465,21 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="A14" s="2">
+        <v>43176</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
@@ -1508,7 +1540,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week8 day1] Work hard, study hard, and pay close attention to time to finish mathematics. The game has been deleted, but it feels a lot easier.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -389,6 +389,15 @@
                 <c:pt idx="12">
                   <c:v>43176</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>43177</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43178</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43179</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -436,6 +445,15 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,6 +526,15 @@
                 <c:pt idx="12">
                   <c:v>43176</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>43177</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43178</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43179</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -554,6 +581,15 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -622,6 +658,15 @@
                 <c:pt idx="12">
                   <c:v>43176</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>43177</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43178</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43179</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -670,15 +715,24 @@
                 <c:pt idx="12">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="79867904"/>
-        <c:axId val="79869824"/>
+        <c:axId val="68268032"/>
+        <c:axId val="68269952"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="79867904"/>
+        <c:axId val="68268032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,14 +809,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79869824"/>
+        <c:crossAx val="68269952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79869824"/>
+        <c:axId val="68269952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,10 +906,15 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79867904"/>
+        <c:crossAx val="68268032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -922,7 +981,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -948,7 +1007,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1240,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1251,7 +1310,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1482,24 +1541,48 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="2">
+        <v>43177</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="2">
+        <v>43178</v>
+      </c>
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="2">
+        <v>43179</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3</v>
+      </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:11">
@@ -1540,7 +1623,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week8 day2] The state of today is very poor, don't think about it. Let's study hard.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -453,7 +453,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -590,7 +590,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,17 +722,17 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="68268032"/>
-        <c:axId val="68269952"/>
+        <c:axId val="64008192"/>
+        <c:axId val="64010112"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="68268032"/>
+        <c:axId val="64008192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,14 +809,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68269952"/>
+        <c:crossAx val="64010112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68269952"/>
+        <c:axId val="64010112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +906,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68268032"/>
+        <c:crossAx val="64008192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -981,7 +981,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1007,7 +1007,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1299,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1310,7 +1310,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1575,13 +1575,13 @@
         <v>43179</v>
       </c>
       <c r="B17" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C17" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E17" s="4"/>
     </row>
@@ -1623,7 +1623,7 @@
     <row r="23" spans="1:11">
       <c r="B23" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>

</xml_diff>

<commit_message>
[week8 day4] cold, uncomfortable, want to cry
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A69A9C4-7555-4AB0-AC50-CE64FE7076CB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="身体状态" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>xy</t>
   </si>
@@ -145,14 +144,18 @@
   </si>
   <si>
     <t>感冒了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">感冒 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,42 +230,42 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -278,18 +281,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -317,7 +310,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -326,12 +319,10 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:radarChart>
         <c:radarStyle val="marker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="0"/>
@@ -354,14 +345,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -371,7 +356,7 @@
             <c:numRef>
               <c:f>身体状态!$A$2:$A$22</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>yyyy/m/d</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>43164</c:v>
@@ -423,6 +408,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>43180</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,10 +472,13 @@
                 <c:pt idx="16">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-28CA-47A6-B8D8-3FE9652FF6B7}"/>
             </c:ext>
@@ -515,14 +506,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -532,7 +517,7 @@
             <c:numRef>
               <c:f>身体状态!$A$2:$A$22</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>yyyy/m/d</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>43164</c:v>
@@ -584,6 +569,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>43180</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -645,10 +633,13 @@
                 <c:pt idx="16">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E2DC-4425-9D9D-76E30BA0122B}"/>
             </c:ext>
@@ -676,14 +667,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -693,7 +678,7 @@
             <c:numRef>
               <c:f>身体状态!$A$2:$A$22</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>yyyy/m/d</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>43164</c:v>
@@ -745,6 +730,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>43180</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,32 +794,27 @@
                 <c:pt idx="16">
                   <c:v>5</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E2DC-4425-9D9D-76E30BA0122B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="64008192"/>
-        <c:axId val="64010112"/>
+        <c:dLbls/>
+        <c:axId val="86229760"/>
+        <c:axId val="86231680"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="64008192"/>
+        <c:axId val="86229760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:title>
@@ -860,7 +843,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -869,9 +852,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -906,19 +888,17 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64010112"/>
+        <c:crossAx val="86231680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64010112"/>
+        <c:axId val="86231680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -960,7 +940,7 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -971,7 +951,6 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1006,7 +985,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64008192"/>
+        <c:crossAx val="86229760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1018,7 +997,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1047,9 +1026,7 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1083,7 +1060,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1109,7 +1086,7 @@
         <xdr:cNvPr id="3" name="图表 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038A3D36-3399-4C22-8358-33970E9B14AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1131,13 +1108,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表2_2" displayName="表2_2" ref="B1:E23" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
-  <autoFilter ref="B1:E22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:E23" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+  <autoFilter ref="B1:E22"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="xy" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="睡觉时间，以10点半为起点" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="心情" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="列1" dataDxfId="4" totalsRowDxfId="0"/>
+    <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="心情" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="3" name="列1" dataDxfId="4" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1398,21 +1375,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.875" style="3" customWidth="1"/>
@@ -1423,7 +1400,7 @@
     <col min="8" max="8" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1440,7 +1417,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>43164</v>
       </c>
@@ -1455,7 +1432,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>43165</v>
       </c>
@@ -1470,7 +1447,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>43166</v>
       </c>
@@ -1485,7 +1462,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>43167</v>
       </c>
@@ -1500,7 +1477,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>43168</v>
       </c>
@@ -1515,7 +1492,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>43169</v>
       </c>
@@ -1532,7 +1509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>43170</v>
       </c>
@@ -1547,7 +1524,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>43171</v>
       </c>
@@ -1562,7 +1539,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>43172</v>
       </c>
@@ -1577,7 +1554,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>43173</v>
       </c>
@@ -1592,7 +1569,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>43174</v>
       </c>
@@ -1607,7 +1584,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>43175</v>
       </c>
@@ -1622,7 +1599,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>43176</v>
       </c>
@@ -1639,7 +1616,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>43177</v>
       </c>
@@ -1654,7 +1631,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>43178</v>
       </c>
@@ -1669,7 +1646,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="2">
         <v>43179</v>
       </c>
@@ -1684,7 +1661,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="2">
         <v>43180</v>
       </c>
@@ -1701,44 +1678,54 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
+      <c r="A19" s="2">
+        <v>43181</v>
+      </c>
+      <c r="B19" s="4">
+        <v>5</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="B23" s="3">
-        <f>SUBTOTAL(109,表2_2[xy])</f>
-        <v>70</v>
+        <f>SUBTOTAL(109,[xy])</f>
+        <v>75</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
@@ -1746,7 +1733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -1757,7 +1744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="3">
         <v>1</v>
       </c>
@@ -1768,7 +1755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -1785,7 +1772,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="3">
         <v>3</v>
       </c>
@@ -1796,7 +1783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="3">
         <v>4</v>
       </c>
@@ -1807,7 +1794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" s="3">
         <v>5</v>
       </c>
@@ -1818,7 +1805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" s="3">
         <v>6</v>
       </c>
@@ -1829,7 +1816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="3">
         <v>7</v>
       </c>
@@ -1840,7 +1827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="3">
         <v>8</v>
       </c>
@@ -1851,7 +1838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="3">
         <v>9</v>
       </c>
@@ -1862,7 +1849,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="3">
         <v>10</v>
       </c>
@@ -1873,7 +1860,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="85.5">
       <c r="A41" s="6" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
[week8 day5] today's goal is to finish the ninth chapter in mathematics.
</commit_message>
<xml_diff>
--- a/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
+++ b/Personal/xueyu/physical status/身体状态记录 - 2018年3月.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>xy</t>
   </si>
@@ -148,6 +148,10 @@
   </si>
   <si>
     <t xml:space="preserve">感冒 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还有一点感冒</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -354,10 +358,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>身体状态!$A$2:$A$22</c:f>
+              <c:f>身体状态!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>yyyy/m/d</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43164</c:v>
                 </c:pt>
@@ -411,16 +415,43 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>43181</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43183</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43184</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43185</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43186</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43187</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43188</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43189</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>身体状态!$C$2:$C$22</c:f>
+              <c:f>身体状态!$C$2:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -474,6 +505,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -515,10 +549,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>身体状态!$A$2:$A$22</c:f>
+              <c:f>身体状态!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>yyyy/m/d</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43164</c:v>
                 </c:pt>
@@ -572,16 +606,43 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>43181</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43183</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43184</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43185</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43186</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43187</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43188</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43189</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>身体状态!$D$2:$D$22</c:f>
+              <c:f>身体状态!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -634,6 +695,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
@@ -676,10 +740,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>身体状态!$A$2:$A$22</c:f>
+              <c:f>身体状态!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>yyyy/m/d</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>43164</c:v>
                 </c:pt>
@@ -733,16 +797,43 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>43181</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43183</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43184</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>43185</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43186</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>43187</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43188</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>43189</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43190</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>身体状态!$B$2:$B$22</c:f>
+              <c:f>身体状态!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -796,6 +887,9 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,12 +900,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="86229760"/>
-        <c:axId val="86231680"/>
+        <c:axId val="89815296"/>
+        <c:axId val="89457024"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="86229760"/>
+        <c:axId val="89815296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,14 +981,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86231680"/>
+        <c:crossAx val="89457024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86231680"/>
+        <c:axId val="89457024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,7 +1078,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86229760"/>
+        <c:crossAx val="89815296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1060,7 +1153,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1078,7 +1171,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>352427</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1108,8 +1201,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:E23" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
-  <autoFilter ref="B1:E22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表2_2" displayName="表2_2" ref="B1:E29" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+  <autoFilter ref="B1:E28"/>
   <tableColumns count="4">
     <tableColumn id="4" name="xy" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="3"/>
     <tableColumn id="1" name="睡觉时间，以10点半为起点" dataDxfId="6" totalsRowDxfId="2"/>
@@ -1383,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1646,7 +1739,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>43179</v>
       </c>
@@ -1661,7 +1754,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>43180</v>
       </c>
@@ -1678,7 +1771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>43181</v>
       </c>
@@ -1695,173 +1788,241 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="2"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="2"/>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>43182</v>
+      </c>
+      <c r="B20" s="4">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>43183</v>
+      </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>43184</v>
+      </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:11">
-      <c r="B23" s="3">
+    <row r="23" spans="1:5">
+      <c r="A23" s="2">
+        <v>43185</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>43186</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>43187</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2">
+        <v>43188</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2">
+        <v>43189</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2">
+        <v>43190</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="3">
         <f>SUBTOTAL(109,[xy])</f>
-        <v>75</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="B28" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="B34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C34" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="3">
+    <row r="35" spans="1:11">
+      <c r="A35" s="3">
         <v>0</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="3">
+    <row r="36" spans="1:11">
+      <c r="A36" s="3">
         <v>1</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="3">
+    <row r="37" spans="1:11">
+      <c r="A37" s="3">
         <v>2</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
         <v>18</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="3">
-        <v>3</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="3">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C38" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3">
+    <row r="39" spans="1:11">
+      <c r="A39" s="3">
         <v>4</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C39" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="3">
+    <row r="40" spans="1:11">
+      <c r="A40" s="3">
         <v>5</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="3">
+    <row r="41" spans="1:11">
+      <c r="A41" s="3">
         <v>6</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C41" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="3">
+    <row r="42" spans="1:11">
+      <c r="A42" s="3">
         <v>7</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="3">
+    <row r="43" spans="1:11">
+      <c r="A43" s="3">
         <v>8</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="3">
+    <row r="44" spans="1:11">
+      <c r="A44" s="3">
         <v>9</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="3">
+    <row r="45" spans="1:11">
+      <c r="A45" s="3">
         <v>10</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C45" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="85.5">
-      <c r="A41" s="6" t="s">
+    <row r="47" spans="1:11" ht="85.5">
+      <c r="A47" s="6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>